<commit_message>
nmv 26 09 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr showObjects="none" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="15" r:id="rId1"/>
-    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId2"/>
+    <sheet name="3.2" sheetId="16" r:id="rId2"/>
+    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="140">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1509,6 +1510,147 @@
   </si>
   <si>
     <t>3.1.11.8 :</t>
+  </si>
+  <si>
+    <t>3.2.1.1 :</t>
+  </si>
+  <si>
+    <t>3.2.1.2 :</t>
+  </si>
+  <si>
+    <t>3.2.1.3 :</t>
+  </si>
+  <si>
+    <t>3.2.2.1 :</t>
+  </si>
+  <si>
+    <t>3.2.2.2 :</t>
+  </si>
+  <si>
+    <t>3.2.2.3 :</t>
+  </si>
+  <si>
+    <t>3.2.3.1 :</t>
+  </si>
+  <si>
+    <t>3.2.3.2 :</t>
+  </si>
+  <si>
+    <t>3.2.3.3 :</t>
+  </si>
+  <si>
+    <t>3.2.3.4 :</t>
+  </si>
+  <si>
+    <t>3.2.4.1 :</t>
+  </si>
+  <si>
+    <t>3.2.4.2 :</t>
+  </si>
+  <si>
+    <t>3.2.4.3 :</t>
+  </si>
+  <si>
+    <t>3.2.4.4 :</t>
+  </si>
+  <si>
+    <t>3.2.4.5 :</t>
+  </si>
+  <si>
+    <t>3.2.5.1 :</t>
+  </si>
+  <si>
+    <t>3.2.5.2 :</t>
+  </si>
+  <si>
+    <t>3.2.5.3 :</t>
+  </si>
+  <si>
+    <t>3.2.5.4 :</t>
+  </si>
+  <si>
+    <t>3.2.5.5 :</t>
+  </si>
+  <si>
+    <t>3.2.5.6 :</t>
+  </si>
+  <si>
+    <t>3.2.5.7 :</t>
+  </si>
+  <si>
+    <t>3.2.6.1 :</t>
+  </si>
+  <si>
+    <t>3.2.6.2 :</t>
+  </si>
+  <si>
+    <t>3.2.6.3 :</t>
+  </si>
+  <si>
+    <t>3.2.7.1 :</t>
+  </si>
+  <si>
+    <t>3.2.7.2 :</t>
+  </si>
+  <si>
+    <t>3.2.7.3 :</t>
+  </si>
+  <si>
+    <t>3.2.8.1 :</t>
+  </si>
+  <si>
+    <t>3.2.8.2 :</t>
+  </si>
+  <si>
+    <t>3.2.8.3 :</t>
+  </si>
+  <si>
+    <t>3.2.8.4 :</t>
+  </si>
+  <si>
+    <t>3.2.8.5 :</t>
+  </si>
+  <si>
+    <t>3.2.8.6 :</t>
+  </si>
+  <si>
+    <t>3.2.9.1 :</t>
+  </si>
+  <si>
+    <t>3.2.9.2 :</t>
+  </si>
+  <si>
+    <t>3.2.9.3 :</t>
+  </si>
+  <si>
+    <t>3.2.9.4 :</t>
+  </si>
+  <si>
+    <t>3.2.9.5 :</t>
+  </si>
+  <si>
+    <t>3.2.9.6 :</t>
+  </si>
+  <si>
+    <t>3.2.9.7 :</t>
+  </si>
+  <si>
+    <t>3.2.10.1 :</t>
+  </si>
+  <si>
+    <t>3.2.10.2 :</t>
+  </si>
+  <si>
+    <t>3.2.11.1 :</t>
+  </si>
+  <si>
+    <t>3.2.11.2 :</t>
+  </si>
+  <si>
+    <t>3.2.11.3 :</t>
+  </si>
+  <si>
+    <t>46</t>
   </si>
 </sst>
 </file>
@@ -2092,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:L44"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45:J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3895,9 +4037,1965 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+      <c r="L2" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="5">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>42</v>
+      </c>
+      <c r="K3" s="5">
+        <v>50</v>
+      </c>
+      <c r="L3" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="5">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>33</v>
+      </c>
+      <c r="K4" s="5">
+        <v>42</v>
+      </c>
+      <c r="L4" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="5">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>36</v>
+      </c>
+      <c r="K5" s="5">
+        <v>50</v>
+      </c>
+      <c r="L5" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="5">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>36</v>
+      </c>
+      <c r="K6" s="5">
+        <v>50</v>
+      </c>
+      <c r="L6" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>42</v>
+      </c>
+      <c r="K7" s="5">
+        <v>53</v>
+      </c>
+      <c r="L7" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="5">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>36</v>
+      </c>
+      <c r="K8" s="5">
+        <v>50</v>
+      </c>
+      <c r="L8" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>40</v>
+      </c>
+      <c r="K9" s="5">
+        <v>50</v>
+      </c>
+      <c r="L9" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="5">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>43</v>
+      </c>
+      <c r="K10" s="5">
+        <v>50</v>
+      </c>
+      <c r="L10" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>4</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>36</v>
+      </c>
+      <c r="K11" s="5">
+        <v>45</v>
+      </c>
+      <c r="L11" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="5">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>7</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>42</v>
+      </c>
+      <c r="K12" s="5">
+        <v>50</v>
+      </c>
+      <c r="L12" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>42</v>
+      </c>
+      <c r="K13" s="5">
+        <v>50</v>
+      </c>
+      <c r="L13" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>3</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>43</v>
+      </c>
+      <c r="K14" s="5">
+        <v>50</v>
+      </c>
+      <c r="L14" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="5">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>4</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>42</v>
+      </c>
+      <c r="K15" s="5">
+        <v>50</v>
+      </c>
+      <c r="L15" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>5</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>27</v>
+      </c>
+      <c r="K16" s="5">
+        <v>33</v>
+      </c>
+      <c r="L16" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="5">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>38</v>
+      </c>
+      <c r="K17" s="5">
+        <v>50</v>
+      </c>
+      <c r="L17" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="5">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>29</v>
+      </c>
+      <c r="K18" s="5">
+        <v>50</v>
+      </c>
+      <c r="L18" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="5">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1</v>
+      </c>
+      <c r="J19" s="5">
+        <v>31</v>
+      </c>
+      <c r="K19" s="5">
+        <v>50</v>
+      </c>
+      <c r="L19" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="5">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>6</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>41</v>
+      </c>
+      <c r="K20" s="5">
+        <v>50</v>
+      </c>
+      <c r="L20" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="5">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>3</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>38</v>
+      </c>
+      <c r="K21" s="5">
+        <v>50</v>
+      </c>
+      <c r="L21" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>3</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>47</v>
+      </c>
+      <c r="K22" s="5">
+        <v>50</v>
+      </c>
+      <c r="L22" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="5">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>24</v>
+      </c>
+      <c r="K23" s="5">
+        <v>44</v>
+      </c>
+      <c r="L23" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>3</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>46</v>
+      </c>
+      <c r="K24" s="5">
+        <v>50</v>
+      </c>
+      <c r="L24" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="5">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>35</v>
+      </c>
+      <c r="K25" s="5">
+        <v>50</v>
+      </c>
+      <c r="L25" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="5">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>5</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5">
+        <v>56</v>
+      </c>
+      <c r="K26" s="5">
+        <v>72</v>
+      </c>
+      <c r="L26" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="5">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>46</v>
+      </c>
+      <c r="K27" s="5">
+        <v>50</v>
+      </c>
+      <c r="L27" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="5">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>4</v>
+      </c>
+      <c r="G28" s="5">
+        <v>4</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>40</v>
+      </c>
+      <c r="K28" s="5">
+        <v>50</v>
+      </c>
+      <c r="L28" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>2</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>67</v>
+      </c>
+      <c r="K29" s="5">
+        <v>72</v>
+      </c>
+      <c r="L29" s="5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="5">
+        <v>14</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5">
+        <v>36</v>
+      </c>
+      <c r="K30" s="5">
+        <v>50</v>
+      </c>
+      <c r="L30" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="5">
+        <v>11</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>6</v>
+      </c>
+      <c r="G31" s="5">
+        <v>2</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <v>33</v>
+      </c>
+      <c r="K31" s="5">
+        <v>50</v>
+      </c>
+      <c r="L31" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="5">
+        <v>8</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>3</v>
+      </c>
+      <c r="G32" s="5">
+        <v>2</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5">
+        <v>40</v>
+      </c>
+      <c r="K32" s="5">
+        <v>50</v>
+      </c>
+      <c r="L32" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="5">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5">
+        <v>39</v>
+      </c>
+      <c r="K33" s="5">
+        <v>50</v>
+      </c>
+      <c r="L33" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="5">
+        <v>7</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>4</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5">
+        <v>40</v>
+      </c>
+      <c r="K34" s="5">
+        <v>50</v>
+      </c>
+      <c r="L34" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>4</v>
+      </c>
+      <c r="G35" s="5">
+        <v>2</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <v>34</v>
+      </c>
+      <c r="K35" s="5">
+        <v>40</v>
+      </c>
+      <c r="L35" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="5">
+        <v>9</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5">
+        <v>41</v>
+      </c>
+      <c r="K36" s="5">
+        <v>50</v>
+      </c>
+      <c r="L36" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="5">
+        <v>13</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <v>37</v>
+      </c>
+      <c r="K37" s="5">
+        <v>50</v>
+      </c>
+      <c r="L37" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="5">
+        <v>9</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>2</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
+        <v>39</v>
+      </c>
+      <c r="K38" s="5">
+        <v>50</v>
+      </c>
+      <c r="L38" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="5">
+        <v>9</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5">
+        <v>40</v>
+      </c>
+      <c r="K39" s="5">
+        <v>50</v>
+      </c>
+      <c r="L39" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="5">
+        <v>15</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>3</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5">
+        <v>35</v>
+      </c>
+      <c r="K40" s="5">
+        <v>50</v>
+      </c>
+      <c r="L40" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="5">
+        <v>7</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5">
+        <v>1</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <v>42</v>
+      </c>
+      <c r="K41" s="5">
+        <v>50</v>
+      </c>
+      <c r="L41" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="5">
+        <v>6</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="5">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5">
+        <v>5</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>50</v>
+      </c>
+      <c r="K42" s="5">
+        <v>58</v>
+      </c>
+      <c r="L42" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="5">
+        <v>17</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
+        <v>33</v>
+      </c>
+      <c r="K43" s="5">
+        <v>50</v>
+      </c>
+      <c r="L43" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="5">
+        <v>15</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <v>2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>45</v>
+      </c>
+      <c r="K44" s="5">
+        <v>63</v>
+      </c>
+      <c r="L44" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="5">
+        <v>8</v>
+      </c>
+      <c r="C45" s="5">
+        <v>2</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <v>6</v>
+      </c>
+      <c r="G45" s="5">
+        <v>4</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1</v>
+      </c>
+      <c r="J45" s="5">
+        <v>38</v>
+      </c>
+      <c r="K45" s="5">
+        <v>50</v>
+      </c>
+      <c r="L45" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="5">
+        <v>3</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>5</v>
+      </c>
+      <c r="G46" s="5">
+        <v>3</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+      <c r="I46" s="5">
+        <v>1</v>
+      </c>
+      <c r="J46" s="5">
+        <v>39</v>
+      </c>
+      <c r="K46" s="5">
+        <v>50</v>
+      </c>
+      <c r="L46" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="5">
+        <v>2</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" s="5">
+        <v>9</v>
+      </c>
+      <c r="G47" s="5">
+        <v>3</v>
+      </c>
+      <c r="H47" s="5">
+        <v>0</v>
+      </c>
+      <c r="I47" s="5">
+        <v>0</v>
+      </c>
+      <c r="J47" s="5">
+        <v>49</v>
+      </c>
+      <c r="K47" s="5">
+        <v>63</v>
+      </c>
+      <c r="L47" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="3">
+        <f>SUM(B2:B47)</f>
+        <v>404</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" ref="C48:L48" si="0">SUM(C2:C47)</f>
+        <v>10</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="0"/>
+        <v>1833</v>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="0"/>
+        <v>2335</v>
+      </c>
+      <c r="L48" s="3">
+        <f t="shared" si="0"/>
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <f>G48</f>
+        <v>134</v>
+      </c>
+      <c r="J49">
+        <f>B48-C48</f>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50">
+        <f>B48</f>
+        <v>404</v>
+      </c>
+      <c r="J50">
+        <f>D48-E48</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51">
+        <v>21</v>
+      </c>
+      <c r="J51">
+        <f>F57</f>
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52">
+        <v>7</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53">
+        <f>SUM(J49:J52)</f>
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f>SUM(F49:F53)</f>
+        <v>566</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f>K48-F54</f>
+        <v>1769</v>
+      </c>
+      <c r="J55">
+        <f>J53-L48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f>F55+F54</f>
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f>F57-K48</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25:J29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nmv 11 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showObjects="none" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr showObjects="none"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAFAA24-3F40-4CDC-9D7E-8841109B6214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="15" r:id="rId1"/>
     <sheet name="3.2" sheetId="16" r:id="rId2"/>
-    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId3"/>
+    <sheet name="3.3" sheetId="17" r:id="rId3"/>
+    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1651,12 +1661,120 @@
   </si>
   <si>
     <t>46</t>
+  </si>
+  <si>
+    <t>3.3.1.1 :</t>
+  </si>
+  <si>
+    <t>3.3.1.2 :</t>
+  </si>
+  <si>
+    <t>3.3.2.1 :</t>
+  </si>
+  <si>
+    <t>3.3.2.2 :</t>
+  </si>
+  <si>
+    <t>3.3.3.1 :</t>
+  </si>
+  <si>
+    <t>3.3.3.2 :</t>
+  </si>
+  <si>
+    <t>3.3.3.3 :</t>
+  </si>
+  <si>
+    <t>3.3.4.1 :</t>
+  </si>
+  <si>
+    <t>3.3.4.2 :</t>
+  </si>
+  <si>
+    <t>3.3.4.3 :</t>
+  </si>
+  <si>
+    <t>3.3.5.1 :</t>
+  </si>
+  <si>
+    <t>3.3.5.2 :</t>
+  </si>
+  <si>
+    <t>3.3.5.3 :</t>
+  </si>
+  <si>
+    <t>3.3.5.4 :</t>
+  </si>
+  <si>
+    <t>3.3.5.5 :</t>
+  </si>
+  <si>
+    <t>3.3.6.1 :</t>
+  </si>
+  <si>
+    <t>3.3.6.2 :</t>
+  </si>
+  <si>
+    <t>3.3.6.3 :</t>
+  </si>
+  <si>
+    <t>3.3.7.1 :</t>
+  </si>
+  <si>
+    <t>3.3.7.2 :</t>
+  </si>
+  <si>
+    <t>3.3.7.3 :</t>
+  </si>
+  <si>
+    <t>3.3.8.1 :</t>
+  </si>
+  <si>
+    <t>3.3.8.2 :</t>
+  </si>
+  <si>
+    <t>3.3.8.3 :</t>
+  </si>
+  <si>
+    <t>3.3.8.4 :</t>
+  </si>
+  <si>
+    <t>3.3.8.5 :</t>
+  </si>
+  <si>
+    <t>3.3.8.6 :</t>
+  </si>
+  <si>
+    <t>3.3.9.1 :</t>
+  </si>
+  <si>
+    <t>3.3.9.2 :</t>
+  </si>
+  <si>
+    <t>3.3.10.1 :</t>
+  </si>
+  <si>
+    <t>3.3.10.2 :</t>
+  </si>
+  <si>
+    <t>3.3.11.1 :</t>
+  </si>
+  <si>
+    <t>3.3.11.2 :</t>
+  </si>
+  <si>
+    <t>3.3.11.3 :</t>
+  </si>
+  <si>
+    <t>3.3.11.4 :</t>
+  </si>
+  <si>
+    <t>3.3.11.5 :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1864,7 +1982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -1951,6 +2069,10 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2231,7 +2353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
@@ -4036,11 +4158,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49:K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5992,7 +6114,1584 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86FB952-AC0C-4941-89B2-B69866530C3F}">
+  <dimension ref="A1:L48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>49</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+      <c r="L2" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>67</v>
+      </c>
+      <c r="K3" s="5">
+        <v>73</v>
+      </c>
+      <c r="L3" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="5">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>33</v>
+      </c>
+      <c r="K4" s="5">
+        <v>50</v>
+      </c>
+      <c r="L4" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>25</v>
+      </c>
+      <c r="K5" s="5">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>49</v>
+      </c>
+      <c r="K6" s="5">
+        <v>50</v>
+      </c>
+      <c r="L6" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>46</v>
+      </c>
+      <c r="K7" s="5">
+        <v>50</v>
+      </c>
+      <c r="L7" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <v>9</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>64</v>
+      </c>
+      <c r="K8" s="5">
+        <v>75</v>
+      </c>
+      <c r="L8" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>46</v>
+      </c>
+      <c r="K9" s="5">
+        <v>50</v>
+      </c>
+      <c r="L9" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>48</v>
+      </c>
+      <c r="K10" s="5">
+        <v>50</v>
+      </c>
+      <c r="L10" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>44</v>
+      </c>
+      <c r="K11" s="5">
+        <v>53</v>
+      </c>
+      <c r="L11" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="5">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>41</v>
+      </c>
+      <c r="K12" s="5">
+        <v>50</v>
+      </c>
+      <c r="L12" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="5">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>43</v>
+      </c>
+      <c r="K13" s="5">
+        <v>50</v>
+      </c>
+      <c r="L13" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>4</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>48</v>
+      </c>
+      <c r="K14" s="5">
+        <v>50</v>
+      </c>
+      <c r="L14" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="5">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>44</v>
+      </c>
+      <c r="K15" s="5">
+        <v>50</v>
+      </c>
+      <c r="L15" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="5">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>5</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>37</v>
+      </c>
+      <c r="K16" s="5">
+        <v>46</v>
+      </c>
+      <c r="L16" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="5">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>45</v>
+      </c>
+      <c r="K17" s="5">
+        <v>50</v>
+      </c>
+      <c r="L17" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="5">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>40</v>
+      </c>
+      <c r="K18" s="5">
+        <v>50</v>
+      </c>
+      <c r="L18" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="5">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>6</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>36</v>
+      </c>
+      <c r="K19" s="5">
+        <v>48</v>
+      </c>
+      <c r="L19" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>6</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>44</v>
+      </c>
+      <c r="K20" s="5">
+        <v>50</v>
+      </c>
+      <c r="L20" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>7</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>47</v>
+      </c>
+      <c r="K21" s="5">
+        <v>50</v>
+      </c>
+      <c r="L21" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>3</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>52</v>
+      </c>
+      <c r="K22" s="5">
+        <v>58</v>
+      </c>
+      <c r="L22" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="5">
+        <v>11</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5">
+        <v>3</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>37</v>
+      </c>
+      <c r="K23" s="5">
+        <v>50</v>
+      </c>
+      <c r="L23" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="5">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>6</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>35</v>
+      </c>
+      <c r="K24" s="5">
+        <v>50</v>
+      </c>
+      <c r="L24" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="5">
+        <v>8</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>3</v>
+      </c>
+      <c r="G25" s="5">
+        <v>3</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>39</v>
+      </c>
+      <c r="K25" s="5">
+        <v>50</v>
+      </c>
+      <c r="L25" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="5">
+        <v>8</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5">
+        <v>42</v>
+      </c>
+      <c r="K26" s="5">
+        <v>50</v>
+      </c>
+      <c r="L26" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="5">
+        <v>12</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>38</v>
+      </c>
+      <c r="K27" s="5">
+        <v>50</v>
+      </c>
+      <c r="L27" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>47</v>
+      </c>
+      <c r="K28" s="5">
+        <v>50</v>
+      </c>
+      <c r="L28" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5">
+        <v>3</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>42</v>
+      </c>
+      <c r="K29" s="5">
+        <v>50</v>
+      </c>
+      <c r="L29" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>6</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5">
+        <v>48</v>
+      </c>
+      <c r="K30" s="5">
+        <v>58</v>
+      </c>
+      <c r="L30" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>7</v>
+      </c>
+      <c r="G31" s="5">
+        <v>8</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5">
+        <v>38</v>
+      </c>
+      <c r="K31" s="5">
+        <v>50</v>
+      </c>
+      <c r="L31" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" s="5">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>6</v>
+      </c>
+      <c r="G32" s="5">
+        <v>2</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>28</v>
+      </c>
+      <c r="K32" s="5">
+        <v>44</v>
+      </c>
+      <c r="L32" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="5">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>4</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>8</v>
+      </c>
+      <c r="G33" s="5">
+        <v>3</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5">
+        <v>36</v>
+      </c>
+      <c r="K33" s="5">
+        <v>50</v>
+      </c>
+      <c r="L33" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="5">
+        <v>9</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>7</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5">
+        <v>36</v>
+      </c>
+      <c r="K34" s="5">
+        <v>50</v>
+      </c>
+      <c r="L34" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="5">
+        <v>9</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>7</v>
+      </c>
+      <c r="G35" s="5">
+        <v>3</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <v>37</v>
+      </c>
+      <c r="K35" s="5">
+        <v>50</v>
+      </c>
+      <c r="L35" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="5">
+        <v>8</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>6</v>
+      </c>
+      <c r="G36" s="5">
+        <v>4</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5">
+        <v>36</v>
+      </c>
+      <c r="K36" s="5">
+        <v>50</v>
+      </c>
+      <c r="L36" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="5">
+        <v>14</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>9</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <v>52</v>
+      </c>
+      <c r="K37" s="5">
+        <v>74</v>
+      </c>
+      <c r="L37" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="34">
+        <v>36</v>
+      </c>
+      <c r="B38" s="33">
+        <f>SUM(B2:B37)</f>
+        <v>238</v>
+      </c>
+      <c r="C38" s="33">
+        <f t="shared" ref="C38:L38" si="0">SUM(C2:C37)</f>
+        <v>14</v>
+      </c>
+      <c r="D38" s="33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E38" s="33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F38" s="33">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="G38" s="33">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="H38" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J38" s="33">
+        <f t="shared" si="0"/>
+        <v>1539</v>
+      </c>
+      <c r="K38" s="33">
+        <f t="shared" si="0"/>
+        <v>1857</v>
+      </c>
+      <c r="L38" s="33">
+        <f t="shared" si="0"/>
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <f>G38</f>
+        <v>108</v>
+      </c>
+      <c r="J39">
+        <f>B38-C38</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <f>B38</f>
+        <v>238</v>
+      </c>
+      <c r="J40">
+        <f>D38-E38</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <f>F47</f>
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43">
+        <f>SUM(J39:J42)</f>
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f>SUM(F39:F43)</f>
+        <v>354</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f>K38-F44</f>
+        <v>1503</v>
+      </c>
+      <c r="J45">
+        <f>J43-L38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f>F45+F44</f>
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f>F47-K38</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6400,7 +8099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="39" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:10" ht="33" x14ac:dyDescent="0.4">
       <c r="B25" s="14" t="s">
         <v>25</v>
       </c>
@@ -6417,7 +8116,7 @@
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="2:10" ht="58.5" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:10" ht="49.5" x14ac:dyDescent="0.4">
       <c r="B26" s="14" t="s">
         <v>27</v>
       </c>
@@ -6434,7 +8133,7 @@
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="2:10" ht="117" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:10" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>29</v>
       </c>
@@ -6451,7 +8150,7 @@
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
     </row>
-    <row r="28" spans="2:10" ht="117" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:10" ht="64.5" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>30</v>
       </c>
@@ -6468,7 +8167,7 @@
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="2:10" ht="117" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:10" ht="99" x14ac:dyDescent="0.4">
       <c r="B29" s="14" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
nmv 26 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAFAA24-3F40-4CDC-9D7E-8841109B6214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BB6369-1C82-47C9-8B64-20AEAEE41804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="15" r:id="rId1"/>
     <sheet name="3.2" sheetId="16" r:id="rId2"/>
     <sheet name="3.3" sheetId="17" r:id="rId3"/>
-    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId4"/>
+    <sheet name="3.4" sheetId="18" r:id="rId4"/>
+    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="222">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1769,6 +1770,144 @@
   </si>
   <si>
     <t>3.3.11.5 :</t>
+  </si>
+  <si>
+    <t>3.4.1.1 :</t>
+  </si>
+  <si>
+    <t>3.4.1.2 :</t>
+  </si>
+  <si>
+    <t>3.4.1.3 :</t>
+  </si>
+  <si>
+    <t>3.4.1.4 :</t>
+  </si>
+  <si>
+    <t>3.4.2.1 :</t>
+  </si>
+  <si>
+    <t>3.4.2.2 :</t>
+  </si>
+  <si>
+    <t>3.4.3.1 :</t>
+  </si>
+  <si>
+    <t>3.4.3.2 :</t>
+  </si>
+  <si>
+    <t>3.4.3.3 :</t>
+  </si>
+  <si>
+    <t>3.4.3.4 :</t>
+  </si>
+  <si>
+    <t>3.4.3.5 :</t>
+  </si>
+  <si>
+    <t>3.4.3.6 :</t>
+  </si>
+  <si>
+    <t>3.4.3.7 :</t>
+  </si>
+  <si>
+    <t>3.4.3.8 :</t>
+  </si>
+  <si>
+    <t>3.4.4.1 :</t>
+  </si>
+  <si>
+    <t>3.4.5.1 :</t>
+  </si>
+  <si>
+    <t>3.4.6.1 :</t>
+  </si>
+  <si>
+    <t>3.4.6.2 :</t>
+  </si>
+  <si>
+    <t>3.4.7.1 :</t>
+  </si>
+  <si>
+    <t>3.4.7.2 :</t>
+  </si>
+  <si>
+    <t>3.4.7.3 :</t>
+  </si>
+  <si>
+    <t>3.4.8.1 :</t>
+  </si>
+  <si>
+    <t>3.4.8.2 :</t>
+  </si>
+  <si>
+    <t>3.4.8.3 :</t>
+  </si>
+  <si>
+    <t>3.4.8.4 :</t>
+  </si>
+  <si>
+    <t>3.4.8.5 :</t>
+  </si>
+  <si>
+    <t>3.4.8.6 :</t>
+  </si>
+  <si>
+    <t>3.4.8.7 :</t>
+  </si>
+  <si>
+    <t>3.4.9.1 :</t>
+  </si>
+  <si>
+    <t>3.4.9.2 :</t>
+  </si>
+  <si>
+    <t>3.4.9.3 :</t>
+  </si>
+  <si>
+    <t>3.4.9.4 :</t>
+  </si>
+  <si>
+    <t>3.4.9.5 :</t>
+  </si>
+  <si>
+    <t>3.4.9.6 :</t>
+  </si>
+  <si>
+    <t>3.4.9.7 :</t>
+  </si>
+  <si>
+    <t>3.4.10.1 :</t>
+  </si>
+  <si>
+    <t>3.4.10.2 :</t>
+  </si>
+  <si>
+    <t>3.4.10.3 :</t>
+  </si>
+  <si>
+    <t>3.4.10.4 :</t>
+  </si>
+  <si>
+    <t>3.4.10.5 :</t>
+  </si>
+  <si>
+    <t>3.4.11.1 :</t>
+  </si>
+  <si>
+    <t>3.4.11.2 :</t>
+  </si>
+  <si>
+    <t>3.4.11.3 :</t>
+  </si>
+  <si>
+    <t>3.4.11.4 :</t>
+  </si>
+  <si>
+    <t>3.4.11.5 :</t>
+  </si>
+  <si>
+    <t>3.4.11.6 :</t>
   </si>
 </sst>
 </file>
@@ -1922,7 +2061,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1978,11 +2117,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -2074,6 +2226,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6117,9 +6277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86FB952-AC0C-4941-89B2-B69866530C3F}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7691,6 +7851,1967 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACADAC5B-3EB0-41C6-B31A-ADA5138A9FF2}">
+  <dimension ref="A1:L58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="5">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>42</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+      <c r="L2" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="5">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>42</v>
+      </c>
+      <c r="K3" s="5">
+        <v>50</v>
+      </c>
+      <c r="L3" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="5">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>41</v>
+      </c>
+      <c r="K4" s="5">
+        <v>50</v>
+      </c>
+      <c r="L4" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="5">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>58</v>
+      </c>
+      <c r="K5" s="5">
+        <v>71</v>
+      </c>
+      <c r="L5" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="5">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>39</v>
+      </c>
+      <c r="K6" s="5">
+        <v>50</v>
+      </c>
+      <c r="L6" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>3</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>54</v>
+      </c>
+      <c r="K7" s="5">
+        <v>63</v>
+      </c>
+      <c r="L7" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>41</v>
+      </c>
+      <c r="K8" s="5">
+        <v>50</v>
+      </c>
+      <c r="L8" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="5">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>40</v>
+      </c>
+      <c r="K9" s="5">
+        <v>50</v>
+      </c>
+      <c r="L9" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>6</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>40</v>
+      </c>
+      <c r="K10" s="5">
+        <v>50</v>
+      </c>
+      <c r="L10" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>42</v>
+      </c>
+      <c r="K11" s="5">
+        <v>50</v>
+      </c>
+      <c r="L11" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="5">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>43</v>
+      </c>
+      <c r="K12" s="5">
+        <v>50</v>
+      </c>
+      <c r="L12" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>47</v>
+      </c>
+      <c r="K13" s="5">
+        <v>50</v>
+      </c>
+      <c r="L13" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="5">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5">
+        <v>44</v>
+      </c>
+      <c r="K14" s="5">
+        <v>50</v>
+      </c>
+      <c r="L14" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>31</v>
+      </c>
+      <c r="K15" s="5">
+        <v>42</v>
+      </c>
+      <c r="L15" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="5">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>4</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>63</v>
+      </c>
+      <c r="K16" s="5">
+        <v>75</v>
+      </c>
+      <c r="L16" s="5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="5">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>58</v>
+      </c>
+      <c r="K17" s="5">
+        <v>67</v>
+      </c>
+      <c r="L17" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" s="5">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>43</v>
+      </c>
+      <c r="K18" s="5">
+        <v>50</v>
+      </c>
+      <c r="L18" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>6</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>49</v>
+      </c>
+      <c r="K19" s="5">
+        <v>68</v>
+      </c>
+      <c r="L19" s="5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="5">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>41</v>
+      </c>
+      <c r="K20" s="5">
+        <v>50</v>
+      </c>
+      <c r="L20" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="5">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>37</v>
+      </c>
+      <c r="K21" s="5">
+        <v>50</v>
+      </c>
+      <c r="L21" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>41</v>
+      </c>
+      <c r="K22" s="5">
+        <v>46</v>
+      </c>
+      <c r="L22" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="5">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>3</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>42</v>
+      </c>
+      <c r="K23" s="5">
+        <v>50</v>
+      </c>
+      <c r="L23" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="5">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>3</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>42</v>
+      </c>
+      <c r="K24" s="5">
+        <v>50</v>
+      </c>
+      <c r="L24" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="5">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>39</v>
+      </c>
+      <c r="K25" s="5">
+        <v>50</v>
+      </c>
+      <c r="L25" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="5">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5">
+        <v>43</v>
+      </c>
+      <c r="K26" s="5">
+        <v>50</v>
+      </c>
+      <c r="L26" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="5">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>40</v>
+      </c>
+      <c r="K27" s="5">
+        <v>50</v>
+      </c>
+      <c r="L27" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="5">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>5</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>39</v>
+      </c>
+      <c r="K28" s="5">
+        <v>50</v>
+      </c>
+      <c r="L28" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="5">
+        <v>9</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>3</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>39</v>
+      </c>
+      <c r="K29" s="5">
+        <v>49</v>
+      </c>
+      <c r="L29" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30" s="5">
+        <v>8</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>5</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5">
+        <v>42</v>
+      </c>
+      <c r="K30" s="5">
+        <v>50</v>
+      </c>
+      <c r="L30" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>6</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <v>45</v>
+      </c>
+      <c r="K31" s="5">
+        <v>50</v>
+      </c>
+      <c r="L31" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
+        <v>4</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>48</v>
+      </c>
+      <c r="K32" s="5">
+        <v>50</v>
+      </c>
+      <c r="L32" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="5">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>3</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5">
+        <v>46</v>
+      </c>
+      <c r="K33" s="5">
+        <v>50</v>
+      </c>
+      <c r="L33" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="5">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>6</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5">
+        <v>46</v>
+      </c>
+      <c r="K34" s="5">
+        <v>50</v>
+      </c>
+      <c r="L34" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35" s="5">
+        <v>10</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <v>40</v>
+      </c>
+      <c r="K35" s="5">
+        <v>50</v>
+      </c>
+      <c r="L35" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="5">
+        <v>11</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>5</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>4</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5">
+        <v>42</v>
+      </c>
+      <c r="K36" s="5">
+        <v>59</v>
+      </c>
+      <c r="L36" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="5">
+        <v>9</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>4</v>
+      </c>
+      <c r="G37" s="5">
+        <v>3</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1</v>
+      </c>
+      <c r="J37" s="5">
+        <v>39</v>
+      </c>
+      <c r="K37" s="5">
+        <v>50</v>
+      </c>
+      <c r="L37" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" s="5">
+        <v>11</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>2</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
+        <v>38</v>
+      </c>
+      <c r="K38" s="5">
+        <v>50</v>
+      </c>
+      <c r="L38" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="5">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5">
+        <v>40</v>
+      </c>
+      <c r="K39" s="5">
+        <v>50</v>
+      </c>
+      <c r="L39" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" s="5">
+        <v>14</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5">
+        <v>36</v>
+      </c>
+      <c r="K40" s="5">
+        <v>50</v>
+      </c>
+      <c r="L40" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B41" s="5">
+        <v>5</v>
+      </c>
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5">
+        <v>1</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+      <c r="G41" s="5">
+        <v>3</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <v>39</v>
+      </c>
+      <c r="K41" s="5">
+        <v>45</v>
+      </c>
+      <c r="L41" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" s="5">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="5">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5">
+        <v>7</v>
+      </c>
+      <c r="G42" s="5">
+        <v>2</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>33</v>
+      </c>
+      <c r="K42" s="5">
+        <v>50</v>
+      </c>
+      <c r="L42" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B43" s="5">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <v>7</v>
+      </c>
+      <c r="G43" s="5">
+        <v>4</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+      <c r="J43" s="5">
+        <v>37</v>
+      </c>
+      <c r="K43" s="5">
+        <v>50</v>
+      </c>
+      <c r="L43" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" s="5">
+        <v>7</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>6</v>
+      </c>
+      <c r="G44" s="5">
+        <v>4</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>38</v>
+      </c>
+      <c r="K44" s="5">
+        <v>50</v>
+      </c>
+      <c r="L44" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" s="5">
+        <v>3</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>7</v>
+      </c>
+      <c r="G45" s="5">
+        <v>2</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1</v>
+      </c>
+      <c r="J45" s="5">
+        <v>41</v>
+      </c>
+      <c r="K45" s="5">
+        <v>50</v>
+      </c>
+      <c r="L45" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B46" s="5">
+        <v>6</v>
+      </c>
+      <c r="C46" s="5">
+        <v>2</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>7</v>
+      </c>
+      <c r="G46" s="5">
+        <v>2</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5">
+        <v>39</v>
+      </c>
+      <c r="K46" s="5">
+        <v>50</v>
+      </c>
+      <c r="L46" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="38">
+        <v>2</v>
+      </c>
+      <c r="C47" s="38">
+        <v>1</v>
+      </c>
+      <c r="D47" s="38">
+        <v>0</v>
+      </c>
+      <c r="E47" s="38">
+        <v>0</v>
+      </c>
+      <c r="F47" s="38">
+        <v>6</v>
+      </c>
+      <c r="G47" s="38">
+        <v>2</v>
+      </c>
+      <c r="H47" s="38">
+        <v>0</v>
+      </c>
+      <c r="I47" s="38">
+        <v>2</v>
+      </c>
+      <c r="J47" s="38">
+        <v>50</v>
+      </c>
+      <c r="K47" s="38">
+        <v>57</v>
+      </c>
+      <c r="L47" s="38">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="37">
+        <v>46</v>
+      </c>
+      <c r="B48" s="37">
+        <f>SUM(B2:B47)</f>
+        <v>366</v>
+      </c>
+      <c r="C48" s="37">
+        <f t="shared" ref="C48:L48" si="0">SUM(C2:C47)</f>
+        <v>12</v>
+      </c>
+      <c r="D48" s="37">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E48" s="37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F48" s="37">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="G48" s="37">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="H48" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="37">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J48" s="37">
+        <f t="shared" si="0"/>
+        <v>1959</v>
+      </c>
+      <c r="K48" s="37">
+        <f t="shared" si="0"/>
+        <v>2392</v>
+      </c>
+      <c r="L48" s="37">
+        <f t="shared" si="0"/>
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <f>G48</f>
+        <v>132</v>
+      </c>
+      <c r="J49">
+        <f>B48-C48</f>
+        <v>354</v>
+      </c>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="36"/>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50">
+        <f>B48</f>
+        <v>366</v>
+      </c>
+      <c r="J50">
+        <f>D48-E48</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51">
+        <v>14</v>
+      </c>
+      <c r="J51">
+        <f>F57</f>
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53">
+        <f>SUM(J49:J52)</f>
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f>SUM(F49:F53)</f>
+        <v>514</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f>K48-F54</f>
+        <v>1878</v>
+      </c>
+      <c r="J55">
+        <f>J53-L48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f>F55+F54</f>
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f>F57-K48</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J30"/>
   <sheetViews>
@@ -7734,7 +9855,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
nmv 08 11 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 3.1 TO 3.5.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr showObjects="none"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BB6369-1C82-47C9-8B64-20AEAEE41804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D465C0AD-D32E-4E47-9551-13FF46D79EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3.1" sheetId="15" r:id="rId1"/>
     <sheet name="3.2" sheetId="16" r:id="rId2"/>
     <sheet name="3.3" sheetId="17" r:id="rId3"/>
     <sheet name="3.4" sheetId="18" r:id="rId4"/>
-    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId5"/>
+    <sheet name="3.5" sheetId="19" r:id="rId5"/>
+    <sheet name="total 3.1 to 3.5" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="259">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1909,12 +1910,123 @@
   <si>
     <t>3.4.11.6 :</t>
   </si>
+  <si>
+    <t>3.5.1.1 :</t>
+  </si>
+  <si>
+    <t>3.5.1.2 :</t>
+  </si>
+  <si>
+    <t>3.5.1.3 :</t>
+  </si>
+  <si>
+    <t>3.5.1.4 :</t>
+  </si>
+  <si>
+    <t>3.5.2.1 :</t>
+  </si>
+  <si>
+    <t>3.5.2.2 :</t>
+  </si>
+  <si>
+    <t>3.5.2.3 :</t>
+  </si>
+  <si>
+    <t>3.5.2.4 :</t>
+  </si>
+  <si>
+    <t>3.5.2.5 :</t>
+  </si>
+  <si>
+    <t>3.5.3.1 :</t>
+  </si>
+  <si>
+    <t>3.5.3.2 :</t>
+  </si>
+  <si>
+    <t>3.5.4.1 :</t>
+  </si>
+  <si>
+    <t>3.5.4.2 :</t>
+  </si>
+  <si>
+    <t>3.5.4.3 :</t>
+  </si>
+  <si>
+    <t>3.5.4.4 :</t>
+  </si>
+  <si>
+    <t>3.5.5.1 :</t>
+  </si>
+  <si>
+    <t>3.5.5.2 :</t>
+  </si>
+  <si>
+    <t>3.5.5.3 :</t>
+  </si>
+  <si>
+    <t>3.5.6.1 :</t>
+  </si>
+  <si>
+    <t>3.5.6.2 :</t>
+  </si>
+  <si>
+    <t>3.5.6.3 :</t>
+  </si>
+  <si>
+    <t>3.5.7.1 :</t>
+  </si>
+  <si>
+    <t>3.5.7.2 :</t>
+  </si>
+  <si>
+    <t>3.5.7.3 :</t>
+  </si>
+  <si>
+    <t>3.5.8.1 :</t>
+  </si>
+  <si>
+    <t>3.5.9.1 :</t>
+  </si>
+  <si>
+    <t>3.5.9.2 :</t>
+  </si>
+  <si>
+    <t>3.5.9.3 :</t>
+  </si>
+  <si>
+    <t>3.5.10.1 :</t>
+  </si>
+  <si>
+    <t>3.5.10.2 :</t>
+  </si>
+  <si>
+    <t>3.5.10.3 :</t>
+  </si>
+  <si>
+    <t>3.5.11.1 :</t>
+  </si>
+  <si>
+    <t>3.5.11.2 :</t>
+  </si>
+  <si>
+    <t>3.5.11.3 :</t>
+  </si>
+  <si>
+    <t>3.5.11.4 :</t>
+  </si>
+  <si>
+    <t>3.5.11.5 :</t>
+  </si>
+  <si>
+    <t>ord</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2061,7 +2173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2130,11 +2242,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -2234,6 +2357,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2517,10 +2643,10 @@
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:J54"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
@@ -2534,7 +2660,7 @@
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="89.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2572,7 +2698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
@@ -2610,7 +2736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -2648,7 +2774,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
@@ -2686,7 +2812,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
@@ -2724,7 +2850,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="5" t="s">
         <v>55</v>
       </c>
@@ -2762,7 +2888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2800,7 +2926,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>57</v>
       </c>
@@ -2838,7 +2964,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="5" t="s">
         <v>58</v>
       </c>
@@ -2876,7 +3002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="5" t="s">
         <v>59</v>
       </c>
@@ -2914,7 +3040,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="5" t="s">
         <v>60</v>
       </c>
@@ -2952,7 +3078,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
@@ -2990,7 +3116,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
@@ -3028,7 +3154,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="5" t="s">
         <v>63</v>
       </c>
@@ -3066,7 +3192,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -3104,7 +3230,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>65</v>
       </c>
@@ -3142,7 +3268,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="5" t="s">
         <v>66</v>
       </c>
@@ -3180,7 +3306,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
@@ -3218,7 +3344,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>68</v>
       </c>
@@ -3256,7 +3382,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>69</v>
       </c>
@@ -3294,7 +3420,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="5" t="s">
         <v>70</v>
       </c>
@@ -3332,7 +3458,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="5" t="s">
         <v>71</v>
       </c>
@@ -3370,7 +3496,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="5" t="s">
         <v>72</v>
       </c>
@@ -3408,7 +3534,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="5" t="s">
         <v>73</v>
       </c>
@@ -3446,7 +3572,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="5" t="s">
         <v>74</v>
       </c>
@@ -3484,7 +3610,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="5" t="s">
         <v>75</v>
       </c>
@@ -3522,7 +3648,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="5" t="s">
         <v>76</v>
       </c>
@@ -3560,7 +3686,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="5" t="s">
         <v>77</v>
       </c>
@@ -3598,7 +3724,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="5" t="s">
         <v>78</v>
       </c>
@@ -3636,7 +3762,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="5" t="s">
         <v>79</v>
       </c>
@@ -3674,7 +3800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="5" t="s">
         <v>80</v>
       </c>
@@ -3712,7 +3838,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="5" t="s">
         <v>81</v>
       </c>
@@ -3750,7 +3876,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="5" t="s">
         <v>82</v>
       </c>
@@ -3788,7 +3914,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="5" t="s">
         <v>83</v>
       </c>
@@ -3826,7 +3952,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="5" t="s">
         <v>84</v>
       </c>
@@ -3864,7 +3990,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="5" t="s">
         <v>85</v>
       </c>
@@ -3902,7 +4028,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="5" t="s">
         <v>86</v>
       </c>
@@ -3940,7 +4066,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="5" t="s">
         <v>87</v>
       </c>
@@ -3978,7 +4104,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="5" t="s">
         <v>88</v>
       </c>
@@ -4016,7 +4142,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75">
       <c r="A40" s="5" t="s">
         <v>89</v>
       </c>
@@ -4054,7 +4180,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="5" t="s">
         <v>90</v>
       </c>
@@ -4092,7 +4218,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="5" t="s">
         <v>91</v>
       </c>
@@ -4130,7 +4256,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="5" t="s">
         <v>92</v>
       </c>
@@ -4168,7 +4294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -4217,7 +4343,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="4"/>
       <c r="E45" t="s">
         <v>12</v>
@@ -4231,7 +4357,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="E46" t="s">
         <v>13</v>
       </c>
@@ -4244,7 +4370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="E47" t="s">
         <v>14</v>
       </c>
@@ -4256,7 +4382,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="E48" t="s">
         <v>15</v>
       </c>
@@ -4267,7 +4393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:10">
       <c r="F49" s="1" t="s">
         <v>16</v>
       </c>
@@ -4276,7 +4402,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:10">
       <c r="F50">
         <f>SUM(F45:F49)</f>
         <v>479</v>
@@ -4285,7 +4411,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:10">
       <c r="F51">
         <f>K44-F50</f>
         <v>1769</v>
@@ -4295,18 +4421,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:10">
       <c r="F52" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:10">
       <c r="F53">
         <f>F51+F50</f>
         <v>2248</v>
       </c>
     </row>
-    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:10">
       <c r="F54">
         <f>F53-K44</f>
         <v>0</v>
@@ -4325,7 +4451,7 @@
       <selection activeCell="E49" sqref="E49:K58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
@@ -4339,7 +4465,7 @@
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="89.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4377,7 +4503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
@@ -4415,7 +4541,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
@@ -4453,7 +4579,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>95</v>
       </c>
@@ -4491,7 +4617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
@@ -4529,7 +4655,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="5" t="s">
         <v>97</v>
       </c>
@@ -4567,7 +4693,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="5" t="s">
         <v>98</v>
       </c>
@@ -4605,7 +4731,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>99</v>
       </c>
@@ -4643,7 +4769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="5" t="s">
         <v>100</v>
       </c>
@@ -4681,7 +4807,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="5" t="s">
         <v>101</v>
       </c>
@@ -4719,7 +4845,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="5" t="s">
         <v>102</v>
       </c>
@@ -4757,7 +4883,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="5" t="s">
         <v>103</v>
       </c>
@@ -4795,7 +4921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="5" t="s">
         <v>104</v>
       </c>
@@ -4833,7 +4959,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="5" t="s">
         <v>105</v>
       </c>
@@ -4871,7 +4997,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="5" t="s">
         <v>106</v>
       </c>
@@ -4909,7 +5035,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>107</v>
       </c>
@@ -4947,7 +5073,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="5" t="s">
         <v>108</v>
       </c>
@@ -4985,7 +5111,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>109</v>
       </c>
@@ -5023,7 +5149,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>110</v>
       </c>
@@ -5061,7 +5187,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>111</v>
       </c>
@@ -5099,7 +5225,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="5" t="s">
         <v>112</v>
       </c>
@@ -5137,7 +5263,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="5" t="s">
         <v>113</v>
       </c>
@@ -5175,7 +5301,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="5" t="s">
         <v>114</v>
       </c>
@@ -5213,7 +5339,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="5" t="s">
         <v>115</v>
       </c>
@@ -5251,7 +5377,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="5" t="s">
         <v>116</v>
       </c>
@@ -5289,7 +5415,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="5" t="s">
         <v>117</v>
       </c>
@@ -5327,7 +5453,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="5" t="s">
         <v>118</v>
       </c>
@@ -5365,7 +5491,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="5" t="s">
         <v>119</v>
       </c>
@@ -5403,7 +5529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="5" t="s">
         <v>120</v>
       </c>
@@ -5441,7 +5567,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="5" t="s">
         <v>121</v>
       </c>
@@ -5479,7 +5605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="5" t="s">
         <v>122</v>
       </c>
@@ -5517,7 +5643,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="5" t="s">
         <v>123</v>
       </c>
@@ -5555,7 +5681,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="5" t="s">
         <v>124</v>
       </c>
@@ -5593,7 +5719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="5" t="s">
         <v>125</v>
       </c>
@@ -5631,7 +5757,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="5" t="s">
         <v>126</v>
       </c>
@@ -5669,7 +5795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="5" t="s">
         <v>127</v>
       </c>
@@ -5707,7 +5833,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="5" t="s">
         <v>128</v>
       </c>
@@ -5745,7 +5871,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="5" t="s">
         <v>129</v>
       </c>
@@ -5783,7 +5909,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="5" t="s">
         <v>130</v>
       </c>
@@ -5821,7 +5947,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75">
       <c r="A40" s="5" t="s">
         <v>131</v>
       </c>
@@ -5859,7 +5985,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="5" t="s">
         <v>132</v>
       </c>
@@ -5897,7 +6023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="5" t="s">
         <v>133</v>
       </c>
@@ -5935,7 +6061,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="5" t="s">
         <v>134</v>
       </c>
@@ -5973,7 +6099,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="5" t="s">
         <v>135</v>
       </c>
@@ -6011,7 +6137,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="5" t="s">
         <v>136</v>
       </c>
@@ -6049,7 +6175,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="5" t="s">
         <v>137</v>
       </c>
@@ -6087,7 +6213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75">
       <c r="A47" s="5" t="s">
         <v>138</v>
       </c>
@@ -6125,7 +6251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="3" t="s">
         <v>139</v>
       </c>
@@ -6174,7 +6300,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:10">
       <c r="E49" t="s">
         <v>12</v>
       </c>
@@ -6187,7 +6313,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:10">
       <c r="E50" t="s">
         <v>13</v>
       </c>
@@ -6200,7 +6326,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:10">
       <c r="E51" t="s">
         <v>14</v>
       </c>
@@ -6212,7 +6338,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:10">
       <c r="E52" t="s">
         <v>15</v>
       </c>
@@ -6223,7 +6349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:10">
       <c r="F53" s="1" t="s">
         <v>16</v>
       </c>
@@ -6232,7 +6358,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:10">
       <c r="F54">
         <f>SUM(F49:F53)</f>
         <v>566</v>
@@ -6241,7 +6367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:10">
       <c r="F55">
         <f>K48-F54</f>
         <v>1769</v>
@@ -6251,18 +6377,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:10">
       <c r="F56" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:10">
       <c r="F57">
         <f>F55+F54</f>
         <v>2335</v>
       </c>
     </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:10">
       <c r="F58">
         <f>F57-K48</f>
         <v>0</v>
@@ -6282,7 +6408,7 @@
       <selection pane="bottomLeft" activeCell="E39" sqref="E39:J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
@@ -6296,7 +6422,7 @@
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="89.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6334,7 +6460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>140</v>
       </c>
@@ -6372,7 +6498,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>141</v>
       </c>
@@ -6410,7 +6536,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>142</v>
       </c>
@@ -6448,7 +6574,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>143</v>
       </c>
@@ -6486,7 +6612,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="5" t="s">
         <v>144</v>
       </c>
@@ -6524,7 +6650,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="5" t="s">
         <v>145</v>
       </c>
@@ -6562,7 +6688,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>146</v>
       </c>
@@ -6600,7 +6726,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="5" t="s">
         <v>147</v>
       </c>
@@ -6638,7 +6764,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="5" t="s">
         <v>148</v>
       </c>
@@ -6676,7 +6802,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="5" t="s">
         <v>149</v>
       </c>
@@ -6714,7 +6840,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="5" t="s">
         <v>150</v>
       </c>
@@ -6752,7 +6878,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="5" t="s">
         <v>151</v>
       </c>
@@ -6790,7 +6916,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="5" t="s">
         <v>152</v>
       </c>
@@ -6828,7 +6954,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="5" t="s">
         <v>153</v>
       </c>
@@ -6866,7 +6992,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>154</v>
       </c>
@@ -6904,7 +7030,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="5" t="s">
         <v>155</v>
       </c>
@@ -6942,7 +7068,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>156</v>
       </c>
@@ -6980,7 +7106,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>157</v>
       </c>
@@ -7018,7 +7144,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>158</v>
       </c>
@@ -7056,7 +7182,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="5" t="s">
         <v>159</v>
       </c>
@@ -7094,7 +7220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="5" t="s">
         <v>160</v>
       </c>
@@ -7132,7 +7258,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="5" t="s">
         <v>161</v>
       </c>
@@ -7170,7 +7296,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="5" t="s">
         <v>162</v>
       </c>
@@ -7208,7 +7334,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="5" t="s">
         <v>163</v>
       </c>
@@ -7246,7 +7372,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="5" t="s">
         <v>164</v>
       </c>
@@ -7284,7 +7410,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="5" t="s">
         <v>165</v>
       </c>
@@ -7322,7 +7448,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="5" t="s">
         <v>166</v>
       </c>
@@ -7360,7 +7486,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="5" t="s">
         <v>167</v>
       </c>
@@ -7398,7 +7524,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="5" t="s">
         <v>168</v>
       </c>
@@ -7436,7 +7562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="5" t="s">
         <v>169</v>
       </c>
@@ -7474,7 +7600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="5" t="s">
         <v>170</v>
       </c>
@@ -7512,7 +7638,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="5" t="s">
         <v>171</v>
       </c>
@@ -7550,7 +7676,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="5" t="s">
         <v>172</v>
       </c>
@@ -7588,7 +7714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="5" t="s">
         <v>173</v>
       </c>
@@ -7626,7 +7752,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="5" t="s">
         <v>174</v>
       </c>
@@ -7664,7 +7790,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="5" t="s">
         <v>175</v>
       </c>
@@ -7702,7 +7828,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="34">
         <v>36</v>
       </c>
@@ -7751,7 +7877,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="E39" t="s">
         <v>12</v>
       </c>
@@ -7764,7 +7890,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="E40" t="s">
         <v>13</v>
       </c>
@@ -7777,7 +7903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="E41" t="s">
         <v>14</v>
       </c>
@@ -7789,7 +7915,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="E42" t="s">
         <v>15</v>
       </c>
@@ -7800,7 +7926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="F43" s="1" t="s">
         <v>16</v>
       </c>
@@ -7809,7 +7935,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="F44">
         <f>SUM(F39:F43)</f>
         <v>354</v>
@@ -7818,7 +7944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="F45">
         <f>K38-F44</f>
         <v>1503</v>
@@ -7828,18 +7954,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="F46" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="F47">
         <f>F45+F44</f>
         <v>1857</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="F48">
         <f>F47-K38</f>
         <v>0</v>
@@ -7854,12 +7980,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACADAC5B-3EB0-41C6-B31A-ADA5138A9FF2}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49:K58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
@@ -7873,7 +7999,7 @@
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="89.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7911,7 +8037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="5" t="s">
         <v>176</v>
       </c>
@@ -7949,7 +8075,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="5" t="s">
         <v>177</v>
       </c>
@@ -7987,7 +8113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75">
       <c r="A4" s="5" t="s">
         <v>178</v>
       </c>
@@ -8025,7 +8151,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>179</v>
       </c>
@@ -8063,7 +8189,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75">
       <c r="A6" s="5" t="s">
         <v>180</v>
       </c>
@@ -8101,7 +8227,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75">
       <c r="A7" s="5" t="s">
         <v>181</v>
       </c>
@@ -8139,7 +8265,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>182</v>
       </c>
@@ -8177,7 +8303,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75">
       <c r="A9" s="5" t="s">
         <v>183</v>
       </c>
@@ -8215,7 +8341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75">
       <c r="A10" s="5" t="s">
         <v>184</v>
       </c>
@@ -8253,7 +8379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="5" t="s">
         <v>185</v>
       </c>
@@ -8291,7 +8417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="5" t="s">
         <v>186</v>
       </c>
@@ -8329,7 +8455,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75">
       <c r="A13" s="5" t="s">
         <v>187</v>
       </c>
@@ -8367,7 +8493,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="5" t="s">
         <v>188</v>
       </c>
@@ -8405,7 +8531,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75">
       <c r="A15" s="5" t="s">
         <v>189</v>
       </c>
@@ -8443,7 +8569,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>190</v>
       </c>
@@ -8481,7 +8607,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="5" t="s">
         <v>191</v>
       </c>
@@ -8519,7 +8645,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>192</v>
       </c>
@@ -8557,7 +8683,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>193</v>
       </c>
@@ -8595,7 +8721,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>194</v>
       </c>
@@ -8633,7 +8759,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="5" t="s">
         <v>195</v>
       </c>
@@ -8671,7 +8797,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="5" t="s">
         <v>196</v>
       </c>
@@ -8709,7 +8835,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75">
       <c r="A23" s="5" t="s">
         <v>197</v>
       </c>
@@ -8747,7 +8873,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="5" t="s">
         <v>198</v>
       </c>
@@ -8785,7 +8911,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75">
       <c r="A25" s="5" t="s">
         <v>199</v>
       </c>
@@ -8823,7 +8949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75">
       <c r="A26" s="5" t="s">
         <v>200</v>
       </c>
@@ -8861,7 +8987,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75">
       <c r="A27" s="5" t="s">
         <v>201</v>
       </c>
@@ -8899,7 +9025,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75">
       <c r="A28" s="5" t="s">
         <v>202</v>
       </c>
@@ -8937,7 +9063,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75">
       <c r="A29" s="5" t="s">
         <v>203</v>
       </c>
@@ -8975,7 +9101,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="5" t="s">
         <v>204</v>
       </c>
@@ -9013,7 +9139,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75">
       <c r="A31" s="5" t="s">
         <v>205</v>
       </c>
@@ -9051,7 +9177,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75">
       <c r="A32" s="5" t="s">
         <v>206</v>
       </c>
@@ -9089,7 +9215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75">
       <c r="A33" s="5" t="s">
         <v>207</v>
       </c>
@@ -9127,7 +9253,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15.75">
       <c r="A34" s="5" t="s">
         <v>208</v>
       </c>
@@ -9165,7 +9291,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75">
       <c r="A35" s="5" t="s">
         <v>209</v>
       </c>
@@ -9203,7 +9329,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75">
       <c r="A36" s="5" t="s">
         <v>210</v>
       </c>
@@ -9241,7 +9367,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="5" t="s">
         <v>211</v>
       </c>
@@ -9279,7 +9405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75">
       <c r="A38" s="5" t="s">
         <v>212</v>
       </c>
@@ -9317,7 +9443,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75">
       <c r="A39" s="5" t="s">
         <v>213</v>
       </c>
@@ -9355,7 +9481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75">
       <c r="A40" s="5" t="s">
         <v>214</v>
       </c>
@@ -9393,7 +9519,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="5" t="s">
         <v>215</v>
       </c>
@@ -9431,7 +9557,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75">
       <c r="A42" s="5" t="s">
         <v>216</v>
       </c>
@@ -9469,7 +9595,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="5" t="s">
         <v>217</v>
       </c>
@@ -9507,7 +9633,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="5" t="s">
         <v>218</v>
       </c>
@@ -9545,7 +9671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="5" t="s">
         <v>219</v>
       </c>
@@ -9583,7 +9709,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75">
       <c r="A46" s="5" t="s">
         <v>220</v>
       </c>
@@ -9621,7 +9747,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75">
       <c r="A47" s="38" t="s">
         <v>221</v>
       </c>
@@ -9659,8 +9785,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="37">
+    <row r="48" spans="1:12" ht="15.75">
+      <c r="A48" s="34">
         <v>46</v>
       </c>
       <c r="B48" s="37">
@@ -9708,7 +9834,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15.75">
       <c r="A49" s="4"/>
       <c r="E49" t="s">
         <v>12</v>
@@ -9724,7 +9850,7 @@
       <c r="K49" s="35"/>
       <c r="L49" s="35"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="15.75">
       <c r="A50" s="36"/>
       <c r="E50" t="s">
         <v>13</v>
@@ -9738,7 +9864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="E51" t="s">
         <v>14</v>
       </c>
@@ -9750,7 +9876,7 @@
         <v>2392</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="E52" t="s">
         <v>15</v>
       </c>
@@ -9761,7 +9887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="F53" s="1" t="s">
         <v>16</v>
       </c>
@@ -9770,7 +9896,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="F54">
         <f>SUM(F49:F53)</f>
         <v>514</v>
@@ -9779,7 +9905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="F55">
         <f>K48-F54</f>
         <v>1878</v>
@@ -9789,18 +9915,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="F56" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="F57">
         <f>F55+F54</f>
         <v>2392</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="F58">
         <f>F57-K48</f>
         <v>0</v>
@@ -9812,14 +9938,1596 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:J30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F44DC0-966F-461C-9161-E0CF6EB788BE}">
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:J29"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75">
+      <c r="A2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="5">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>33</v>
+      </c>
+      <c r="K2" s="5">
+        <v>50</v>
+      </c>
+      <c r="L2" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75">
+      <c r="A3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="5">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>39</v>
+      </c>
+      <c r="K3" s="5">
+        <v>50</v>
+      </c>
+      <c r="L3" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75">
+      <c r="A4" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="5">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>34</v>
+      </c>
+      <c r="K4" s="5">
+        <v>50</v>
+      </c>
+      <c r="L4" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75">
+      <c r="A5" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="5">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>58</v>
+      </c>
+      <c r="K5" s="5">
+        <v>75</v>
+      </c>
+      <c r="L5" s="5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75">
+      <c r="A6" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="5">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>41</v>
+      </c>
+      <c r="K6" s="5">
+        <v>50</v>
+      </c>
+      <c r="L6" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75">
+      <c r="A7" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>47</v>
+      </c>
+      <c r="K7" s="5">
+        <v>50</v>
+      </c>
+      <c r="L7" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75">
+      <c r="A8" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>43</v>
+      </c>
+      <c r="K8" s="5">
+        <v>50</v>
+      </c>
+      <c r="L8" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75">
+      <c r="A9" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>40</v>
+      </c>
+      <c r="K9" s="5">
+        <v>50</v>
+      </c>
+      <c r="L9" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75">
+      <c r="A10" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>20</v>
+      </c>
+      <c r="K10" s="5">
+        <v>30</v>
+      </c>
+      <c r="L10" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75">
+      <c r="A11" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="5">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>3</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>43</v>
+      </c>
+      <c r="K11" s="5">
+        <v>50</v>
+      </c>
+      <c r="L11" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75">
+      <c r="A12" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="5">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>3</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>37</v>
+      </c>
+      <c r="K12" s="5">
+        <v>46</v>
+      </c>
+      <c r="L12" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75">
+      <c r="A13" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>6</v>
+      </c>
+      <c r="G13" s="5">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>36</v>
+      </c>
+      <c r="K13" s="5">
+        <v>50</v>
+      </c>
+      <c r="L13" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75">
+      <c r="A14" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="5">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5">
+        <v>33</v>
+      </c>
+      <c r="K14" s="5">
+        <v>50</v>
+      </c>
+      <c r="L14" s="5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
+      <c r="A15" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="5">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>3</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>41</v>
+      </c>
+      <c r="K15" s="5">
+        <v>50</v>
+      </c>
+      <c r="L15" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
+      <c r="A16" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="5">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
+        <v>3</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>36</v>
+      </c>
+      <c r="K16" s="5">
+        <v>43</v>
+      </c>
+      <c r="L16" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
+      <c r="A17" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>43</v>
+      </c>
+      <c r="K17" s="5">
+        <v>50</v>
+      </c>
+      <c r="L17" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75">
+      <c r="A18" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
+      <c r="G18" s="5">
+        <v>5</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5">
+        <v>44</v>
+      </c>
+      <c r="K18" s="5">
+        <v>50</v>
+      </c>
+      <c r="L18" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B19" s="5">
+        <v>8</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>38</v>
+      </c>
+      <c r="K19" s="5">
+        <v>51</v>
+      </c>
+      <c r="L19" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
+      <c r="A20" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="5">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>6</v>
+      </c>
+      <c r="G20" s="5">
+        <v>6</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>39</v>
+      </c>
+      <c r="K20" s="5">
+        <v>50</v>
+      </c>
+      <c r="L20" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
+      <c r="A21" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B21" s="5">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>40</v>
+      </c>
+      <c r="K21" s="5">
+        <v>50</v>
+      </c>
+      <c r="L21" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75">
+      <c r="A22" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>4</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>24</v>
+      </c>
+      <c r="K22" s="5">
+        <v>30</v>
+      </c>
+      <c r="L22" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
+      <c r="A23" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" s="5">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>4</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>45</v>
+      </c>
+      <c r="K23" s="5">
+        <v>50</v>
+      </c>
+      <c r="L23" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75">
+      <c r="A24" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="5">
+        <v>6</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>43</v>
+      </c>
+      <c r="K24" s="5">
+        <v>50</v>
+      </c>
+      <c r="L24" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75">
+      <c r="A25" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" s="5">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>6</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>55</v>
+      </c>
+      <c r="K25" s="5">
+        <v>67</v>
+      </c>
+      <c r="L25" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75">
+      <c r="A26" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" s="5">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>3</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5">
+        <v>46</v>
+      </c>
+      <c r="K26" s="5">
+        <v>64</v>
+      </c>
+      <c r="L26" s="5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75">
+      <c r="A27" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>43</v>
+      </c>
+      <c r="K27" s="5">
+        <v>50</v>
+      </c>
+      <c r="L27" s="5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75">
+      <c r="A28" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" s="5">
+        <v>9</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>41</v>
+      </c>
+      <c r="K28" s="5">
+        <v>50</v>
+      </c>
+      <c r="L28" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75">
+      <c r="A29" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29" s="5">
+        <v>9</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>33</v>
+      </c>
+      <c r="K29" s="5">
+        <v>43</v>
+      </c>
+      <c r="L29" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75">
+      <c r="A30" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>3</v>
+      </c>
+      <c r="G30" s="5">
+        <v>4</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5">
+        <v>42</v>
+      </c>
+      <c r="K30" s="5">
+        <v>50</v>
+      </c>
+      <c r="L30" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75">
+      <c r="A31" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" s="5">
+        <v>8</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>2</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <v>42</v>
+      </c>
+      <c r="K31" s="5">
+        <v>50</v>
+      </c>
+      <c r="L31" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75">
+      <c r="A32" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" s="5">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>25</v>
+      </c>
+      <c r="K32" s="5">
+        <v>37</v>
+      </c>
+      <c r="L32" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75">
+      <c r="A33" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="5">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>8</v>
+      </c>
+      <c r="G33" s="5">
+        <v>3</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5">
+        <v>39</v>
+      </c>
+      <c r="K33" s="5">
+        <v>50</v>
+      </c>
+      <c r="L33" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75">
+      <c r="A34" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B34" s="5">
+        <v>10</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>6</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5">
+        <v>35</v>
+      </c>
+      <c r="K34" s="5">
+        <v>50</v>
+      </c>
+      <c r="L34" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75">
+      <c r="A35" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>8</v>
+      </c>
+      <c r="G35" s="5">
+        <v>4</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <v>40</v>
+      </c>
+      <c r="K35" s="5">
+        <v>50</v>
+      </c>
+      <c r="L35" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75">
+      <c r="A36" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B36" s="5">
+        <v>11</v>
+      </c>
+      <c r="C36" s="5">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>10</v>
+      </c>
+      <c r="G36" s="5">
+        <v>7</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1</v>
+      </c>
+      <c r="J36" s="5">
+        <v>35</v>
+      </c>
+      <c r="K36" s="5">
+        <v>50</v>
+      </c>
+      <c r="L36" s="5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75">
+      <c r="A37" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" s="5">
+        <v>8</v>
+      </c>
+      <c r="C37" s="5">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>10</v>
+      </c>
+      <c r="G37" s="5">
+        <v>2</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <v>39</v>
+      </c>
+      <c r="K37" s="5">
+        <v>54</v>
+      </c>
+      <c r="L37" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75">
+      <c r="A38" s="34">
+        <v>36</v>
+      </c>
+      <c r="B38" s="37">
+        <f>SUM(B2:B37)</f>
+        <v>299</v>
+      </c>
+      <c r="C38" s="37">
+        <f t="shared" ref="C38:L38" si="0">SUM(C2:C37)</f>
+        <v>25</v>
+      </c>
+      <c r="D38" s="37">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E38" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="37">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="G38" s="37">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="H38" s="37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="37">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J38" s="37">
+        <f t="shared" si="0"/>
+        <v>1412</v>
+      </c>
+      <c r="K38" s="37">
+        <f t="shared" si="0"/>
+        <v>1790</v>
+      </c>
+      <c r="L38" s="37">
+        <f t="shared" si="0"/>
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75">
+      <c r="A39" s="4"/>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <f>G38</f>
+        <v>113</v>
+      </c>
+      <c r="J39">
+        <f>B38-C38</f>
+        <v>274</v>
+      </c>
+      <c r="K39" s="35"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <f>B38</f>
+        <v>299</v>
+      </c>
+      <c r="J40">
+        <f>D38-E38</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="J41">
+        <f>F47</f>
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43">
+        <f>SUM(J39:J42)</f>
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="F44">
+        <f>SUM(F39:F43)</f>
+        <v>420</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="E45" t="s">
+        <v>258</v>
+      </c>
+      <c r="F45">
+        <f>K38-F44</f>
+        <v>1370</v>
+      </c>
+      <c r="J45">
+        <f>J43-L38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="F46" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="F47">
+        <f>F45+F44</f>
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="F48">
+        <f>F47-K38</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
@@ -9832,7 +11540,7 @@
     <col min="10" max="10" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="60.75" customHeight="1" thickBot="1">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -9855,7 +11563,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="89.25">
       <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
@@ -9882,7 +11590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="28.5">
       <c r="B3" s="14" t="s">
         <v>25</v>
       </c>
@@ -9892,14 +11600,27 @@
       <c r="D3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="E3" s="15">
+        <v>1769</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1769</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1503</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1878</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1370</v>
+      </c>
+      <c r="J3" s="15">
+        <f>SUM(E3:I3)</f>
+        <v>8289</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="28.5">
       <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
@@ -9909,14 +11630,27 @@
       <c r="D4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="2:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="15">
+        <v>123</v>
+      </c>
+      <c r="F4" s="15">
+        <v>134</v>
+      </c>
+      <c r="G4" s="15">
+        <v>108</v>
+      </c>
+      <c r="H4" s="15">
+        <v>132</v>
+      </c>
+      <c r="I4" s="15">
+        <v>113</v>
+      </c>
+      <c r="J4" s="15">
+        <f>SUM(E4:I4)</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="42.75">
       <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
@@ -9926,14 +11660,27 @@
       <c r="D5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="2:10" ht="41.25" x14ac:dyDescent="0.25">
+      <c r="E5" s="15">
+        <v>339</v>
+      </c>
+      <c r="F5" s="15">
+        <v>404</v>
+      </c>
+      <c r="G5" s="15">
+        <v>238</v>
+      </c>
+      <c r="H5" s="15">
+        <v>366</v>
+      </c>
+      <c r="I5" s="15">
+        <v>299</v>
+      </c>
+      <c r="J5" s="15">
+        <f>SUM(E5:I5)</f>
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="41.25">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -9943,14 +11690,27 @@
       <c r="D6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="2:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="15">
+        <v>8</v>
+      </c>
+      <c r="F6" s="15">
+        <v>21</v>
+      </c>
+      <c r="G6" s="15">
+        <v>4</v>
+      </c>
+      <c r="H6" s="15">
+        <v>14</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1</v>
+      </c>
+      <c r="J6" s="15">
+        <f>SUM(E6:I6)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="42.75">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
@@ -9960,14 +11720,27 @@
       <c r="D7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="15">
+        <v>9</v>
+      </c>
+      <c r="F7" s="15">
+        <v>7</v>
+      </c>
+      <c r="G7" s="15">
+        <v>4</v>
+      </c>
+      <c r="H7" s="15">
+        <v>2</v>
+      </c>
+      <c r="I7" s="15">
+        <v>7</v>
+      </c>
+      <c r="J7" s="15">
+        <f>SUM(E7:I7)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="18" t="s">
@@ -9975,33 +11748,37 @@
       </c>
       <c r="E8" s="19">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>2248</v>
       </c>
       <c r="F8" s="19">
         <f t="shared" ref="F8:J8" si="0">SUM(F3:F7)</f>
-        <v>0</v>
+        <v>2335</v>
       </c>
       <c r="G8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1857</v>
       </c>
       <c r="H8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2392</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1790</v>
       </c>
       <c r="J8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>10622</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
       <c r="E9" s="1"/>
-    </row>
-    <row r="12" spans="2:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="39">
+        <f>SUM(E8:I8)-J8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="51.75" thickBot="1">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -10024,7 +11801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="102">
       <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
@@ -10051,7 +11828,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="28.5">
       <c r="B14" s="14" t="s">
         <v>25</v>
       </c>
@@ -10061,14 +11838,27 @@
       <c r="D14" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="2:10" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="E14" s="15">
+        <v>1769</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1769</v>
+      </c>
+      <c r="G14" s="15">
+        <v>1503</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1878</v>
+      </c>
+      <c r="I14" s="15">
+        <v>1370</v>
+      </c>
+      <c r="J14" s="15">
+        <f>SUM(E14:I14)</f>
+        <v>8289</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="49.5">
       <c r="B15" s="14" t="s">
         <v>27</v>
       </c>
@@ -10078,14 +11868,27 @@
       <c r="D15" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="2:10" ht="66" x14ac:dyDescent="0.35">
+      <c r="E15" s="15">
+        <v>123</v>
+      </c>
+      <c r="F15" s="15">
+        <v>134</v>
+      </c>
+      <c r="G15" s="15">
+        <v>108</v>
+      </c>
+      <c r="H15" s="15">
+        <v>132</v>
+      </c>
+      <c r="I15" s="15">
+        <v>113</v>
+      </c>
+      <c r="J15" s="15">
+        <f>SUM(E15:I15)</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="66">
       <c r="B16" s="14" t="s">
         <v>29</v>
       </c>
@@ -10095,14 +11898,27 @@
       <c r="D16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="2:10" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="E16" s="15">
+        <v>339</v>
+      </c>
+      <c r="F16" s="15">
+        <v>404</v>
+      </c>
+      <c r="G16" s="15">
+        <v>238</v>
+      </c>
+      <c r="H16" s="15">
+        <v>366</v>
+      </c>
+      <c r="I16" s="15">
+        <v>299</v>
+      </c>
+      <c r="J16" s="15">
+        <f>SUM(E16:I16)</f>
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="103.5">
       <c r="B17" s="14" t="s">
         <v>30</v>
       </c>
@@ -10112,14 +11928,27 @@
       <c r="D17" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="2:10" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="E17" s="15">
+        <v>8</v>
+      </c>
+      <c r="F17" s="15">
+        <v>21</v>
+      </c>
+      <c r="G17" s="15">
+        <v>4</v>
+      </c>
+      <c r="H17" s="15">
+        <v>14</v>
+      </c>
+      <c r="I17" s="15">
+        <v>1</v>
+      </c>
+      <c r="J17" s="15">
+        <f>SUM(E17:I17)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="103.5">
       <c r="B18" s="14" t="s">
         <v>32</v>
       </c>
@@ -10129,14 +11958,27 @@
       <c r="D18" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E18" s="15">
+        <v>9</v>
+      </c>
+      <c r="F18" s="15">
+        <v>7</v>
+      </c>
+      <c r="G18" s="15">
+        <v>4</v>
+      </c>
+      <c r="H18" s="15">
+        <v>2</v>
+      </c>
+      <c r="I18" s="15">
+        <v>7</v>
+      </c>
+      <c r="J18" s="15">
+        <f>SUM(E18:I18)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18" t="s">
@@ -10144,33 +11986,37 @@
       </c>
       <c r="E19" s="19">
         <f>SUM(E14:E18)</f>
-        <v>0</v>
+        <v>2248</v>
       </c>
       <c r="F19" s="19">
         <f t="shared" ref="F19:J19" si="1">SUM(F14:F18)</f>
-        <v>0</v>
+        <v>2335</v>
       </c>
       <c r="G19" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1857</v>
       </c>
       <c r="H19" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2392</v>
       </c>
       <c r="I19" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1790</v>
       </c>
       <c r="J19" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="22.5" x14ac:dyDescent="0.45">
+        <v>10622</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="22.5">
       <c r="D20" s="22"/>
-    </row>
-    <row r="23" spans="2:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="39">
+        <f>SUM(E19:I19)-J19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="51.75" thickBot="1">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -10193,7 +12039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="102">
       <c r="B24" s="8" t="s">
         <v>18</v>
       </c>
@@ -10220,7 +12066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="33" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:10" ht="28.5">
       <c r="B25" s="14" t="s">
         <v>25</v>
       </c>
@@ -10230,14 +12076,27 @@
       <c r="D25" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="2:10" ht="49.5" x14ac:dyDescent="0.4">
+      <c r="E25" s="15">
+        <v>1769</v>
+      </c>
+      <c r="F25" s="15">
+        <v>1769</v>
+      </c>
+      <c r="G25" s="15">
+        <v>1503</v>
+      </c>
+      <c r="H25" s="15">
+        <v>1878</v>
+      </c>
+      <c r="I25" s="15">
+        <v>1370</v>
+      </c>
+      <c r="J25" s="15">
+        <f>SUM(E25:I25)</f>
+        <v>8289</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="39">
       <c r="B26" s="14" t="s">
         <v>27</v>
       </c>
@@ -10247,14 +12106,27 @@
       <c r="D26" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="2:10" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="E26" s="15">
+        <v>123</v>
+      </c>
+      <c r="F26" s="15">
+        <v>134</v>
+      </c>
+      <c r="G26" s="15">
+        <v>108</v>
+      </c>
+      <c r="H26" s="15">
+        <v>132</v>
+      </c>
+      <c r="I26" s="15">
+        <v>113</v>
+      </c>
+      <c r="J26" s="15">
+        <f>SUM(E26:I26)</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="77.25">
       <c r="B27" s="14" t="s">
         <v>29</v>
       </c>
@@ -10264,14 +12136,27 @@
       <c r="D27" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-    </row>
-    <row r="28" spans="2:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="E27" s="15">
+        <v>339</v>
+      </c>
+      <c r="F27" s="15">
+        <v>404</v>
+      </c>
+      <c r="G27" s="15">
+        <v>238</v>
+      </c>
+      <c r="H27" s="15">
+        <v>366</v>
+      </c>
+      <c r="I27" s="15">
+        <v>299</v>
+      </c>
+      <c r="J27" s="15">
+        <f>SUM(E27:I27)</f>
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="64.5">
       <c r="B28" s="14" t="s">
         <v>30</v>
       </c>
@@ -10281,14 +12166,27 @@
       <c r="D28" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-    </row>
-    <row r="29" spans="2:10" ht="99" x14ac:dyDescent="0.4">
+      <c r="E28" s="15">
+        <v>8</v>
+      </c>
+      <c r="F28" s="15">
+        <v>21</v>
+      </c>
+      <c r="G28" s="15">
+        <v>4</v>
+      </c>
+      <c r="H28" s="15">
+        <v>14</v>
+      </c>
+      <c r="I28" s="15">
+        <v>1</v>
+      </c>
+      <c r="J28" s="15">
+        <f>SUM(E28:I28)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="77.25">
       <c r="B29" s="14" t="s">
         <v>32</v>
       </c>
@@ -10298,14 +12196,27 @@
       <c r="D29" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E29" s="15">
+        <v>9</v>
+      </c>
+      <c r="F29" s="15">
+        <v>7</v>
+      </c>
+      <c r="G29" s="15">
+        <v>4</v>
+      </c>
+      <c r="H29" s="15">
+        <v>2</v>
+      </c>
+      <c r="I29" s="15">
+        <v>7</v>
+      </c>
+      <c r="J29" s="15">
+        <f>SUM(E29:I29)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="18" t="s">
@@ -10313,26 +12224,32 @@
       </c>
       <c r="E30" s="19">
         <f>SUM(E25:E29)</f>
-        <v>0</v>
+        <v>2248</v>
       </c>
       <c r="F30" s="19">
         <f t="shared" ref="F30:J30" si="2">SUM(F25:F29)</f>
-        <v>0</v>
+        <v>2335</v>
       </c>
       <c r="G30" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1857</v>
       </c>
       <c r="H30" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2392</v>
       </c>
       <c r="I30" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1790</v>
       </c>
       <c r="J30" s="19">
         <f t="shared" si="2"/>
+        <v>10622</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="J31" s="39">
+        <f>SUM(E30:I30)-J30</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>